<commit_message>
updated with all instruction codes
</commit_message>
<xml_diff>
--- a/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
+++ b/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project1\single_cycle_MIPS_processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F9AED69-ADF6-4142-87E1-4E4CB6A3BCFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B447056-6CB6-4FE8-BA9C-09D5D872B44E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
+    <workbookView xWindow="1092" yWindow="-276" windowWidth="17280" windowHeight="8964" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>Instruction</t>
   </si>
@@ -197,6 +197,141 @@
       </rPr>
       <t>[the alu will perform an add of A and B]</t>
     </r>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>addiu</t>
+  </si>
+  <si>
+    <t>addu</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>andi</t>
+  </si>
+  <si>
+    <t>lui</t>
+  </si>
+  <si>
+    <t>lw</t>
+  </si>
+  <si>
+    <t>nor</t>
+  </si>
+  <si>
+    <t>xor</t>
+  </si>
+  <si>
+    <t>xori</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>ori</t>
+  </si>
+  <si>
+    <t>slt</t>
+  </si>
+  <si>
+    <t>slti</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t>srl</t>
+  </si>
+  <si>
+    <t>sra</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>subu</t>
+  </si>
+  <si>
+    <t>beq</t>
+  </si>
+  <si>
+    <t>bne</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>jal</t>
+  </si>
+  <si>
+    <t>"000000"</t>
+  </si>
+  <si>
+    <t>"001001"</t>
+  </si>
+  <si>
+    <t>"100000"</t>
+  </si>
+  <si>
+    <t>"100100"</t>
+  </si>
+  <si>
+    <t>"100001"</t>
+  </si>
+  <si>
+    <t>"001100"</t>
+  </si>
+  <si>
+    <t>"001111"</t>
+  </si>
+  <si>
+    <t>"100011"</t>
+  </si>
+  <si>
+    <t>"100111"</t>
+  </si>
+  <si>
+    <t>"100110"</t>
+  </si>
+  <si>
+    <t>"100101"</t>
+  </si>
+  <si>
+    <t>"001110"</t>
+  </si>
+  <si>
+    <t>"001101"</t>
+  </si>
+  <si>
+    <t>"101010"</t>
+  </si>
+  <si>
+    <t>"001010"</t>
+  </si>
+  <si>
+    <t>"000010"</t>
+  </si>
+  <si>
+    <t>"000011"</t>
+  </si>
+  <si>
+    <t>"101011"</t>
+  </si>
+  <si>
+    <t>"100010"</t>
+  </si>
+  <si>
+    <t>"000100"</t>
+  </si>
+  <si>
+    <t>"000101"</t>
   </si>
 </sst>
 </file>
@@ -240,13 +375,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,13 +706,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC2FCD1-6A91-3E43-87BE-182EA48A4800}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -592,34 +730,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
@@ -672,6 +810,270 @@
       </c>
       <c r="J3" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating alu and tb_alu
</commit_message>
<xml_diff>
--- a/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
+++ b/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project1\single_cycle_MIPS_processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC8B2CB-7BE4-4B57-9997-C572329488FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5832ED5-6CF2-43F7-958A-26FE88F08BC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
+    <workbookView xWindow="20565" yWindow="6360" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="139">
   <si>
     <t>Instruction</t>
   </si>
@@ -962,6 +962,9 @@
   </si>
   <si>
     <t>1001 B(rt) &lt;&lt; shamt (needs implementation)</t>
+  </si>
+  <si>
+    <t>Tested and Working?</t>
   </si>
 </sst>
 </file>
@@ -2418,19 +2421,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D515F8C6-F732-4239-8790-C00BB6FBEA93}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.3984375" customWidth="1"/>
     <col min="2" max="2" width="17.69921875" customWidth="1"/>
+    <col min="7" max="7" width="19.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2439,15 +2443,18 @@
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="F2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2464,7 +2471,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2481,7 +2488,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2498,7 +2505,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2515,7 +2522,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2532,7 +2539,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2549,7 +2556,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2566,7 +2573,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2583,7 +2590,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2600,7 +2607,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2617,7 +2624,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2634,7 +2641,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2647,16 +2654,22 @@
       <c r="E14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2740,9 +2753,6 @@
       <c r="B23" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F23" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -2750,9 +2760,6 @@
       </c>
       <c r="B24" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="F24" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fully tested alu (otherthan add/sub)
</commit_message>
<xml_diff>
--- a/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
+++ b/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project1\single_cycle_MIPS_processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5832ED5-6CF2-43F7-958A-26FE88F08BC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6613C98-6A3D-41F2-8DFD-8FD606A08232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20565" yWindow="6360" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="139">
   <si>
     <t>Instruction</t>
   </si>
@@ -1378,7 +1378,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
@@ -2424,7 +2424,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2470,6 +2470,9 @@
       <c r="F3" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2487,6 +2490,9 @@
       <c r="F4" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2504,6 +2510,9 @@
       <c r="F5" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G5" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2521,6 +2530,9 @@
       <c r="F6" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G6" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2538,6 +2550,9 @@
       <c r="F7" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G7" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2555,6 +2570,9 @@
       <c r="F8" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2572,6 +2590,9 @@
       <c r="F9" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G9" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2589,6 +2610,9 @@
       <c r="F10" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G10" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2606,6 +2630,9 @@
       <c r="F11" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G11" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2623,6 +2650,9 @@
       <c r="F12" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2640,6 +2670,9 @@
       <c r="F13" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G13" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2657,6 +2690,9 @@
       <c r="F14" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G14" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" s="7" t="s">
@@ -2668,6 +2704,9 @@
       <c r="F15" s="7" t="s">
         <v>135</v>
       </c>
+      <c r="G15" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2693,9 +2732,7 @@
       <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>135</v>
-      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -2710,9 +2747,7 @@
       <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>135</v>
-      </c>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">

</xml_diff>

<commit_message>
Added ALU into Processor File
</commit_message>
<xml_diff>
--- a/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
+++ b/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project1\single_cycle_MIPS_processor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\school\CPRE381Project1\single_cycle_MIPS_processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6613C98-6A3D-41F2-8DFD-8FD606A08232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2D8B2F-9DFC-410B-9EA6-8CD32EA578D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
+    <workbookView xWindow="31680" yWindow="2880" windowWidth="21600" windowHeight="11325" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="141">
   <si>
     <t>Instruction</t>
   </si>
@@ -965,13 +965,19 @@
   </si>
   <si>
     <t>Tested and Working?</t>
+  </si>
+  <si>
+    <t>halt</t>
+  </si>
+  <si>
+    <t>01 0100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1000,6 +1006,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1034,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1060,6 +1072,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1375,13 +1390,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC2FCD1-6A91-3E43-87BE-182EA48A4800}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2406,6 +2421,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -2423,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D515F8C6-F732-4239-8790-C00BB6FBEA93}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated alu to add sub/add
</commit_message>
<xml_diff>
--- a/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
+++ b/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\school\CPRE381Project1\single_cycle_MIPS_processor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project1\single_cycle_MIPS_processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0378E9B3-6005-4622-A1C7-1BAB475392C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEEC4BF-8026-490A-93B2-F3A78C52BC54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38640" yWindow="2640" windowWidth="17445" windowHeight="11325" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="143">
   <si>
     <t>Instruction</t>
   </si>
@@ -2453,7 +2453,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2748,7 +2748,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2761,9 +2761,14 @@
       <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2776,9 +2781,14 @@
       <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2786,7 +2796,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2794,7 +2804,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2802,7 +2812,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2810,7 +2820,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2818,7 +2828,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2826,7 +2836,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2834,7 +2844,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2842,7 +2852,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2850,7 +2860,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completing tb for part 2c
</commit_message>
<xml_diff>
--- a/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
+++ b/single_cycle_MIPS_processor/Proj1_control_signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project1\single_cycle_MIPS_processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682FE05B-7AE5-48CC-A13B-C838BF3EE1CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2555D6-503F-4F75-B271-D11B5433FB82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -960,13 +960,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC2FCD1-6A91-3E43-87BE-182EA48A4800}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+    <sheetView zoomScale="102" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1309,34 +1309,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
         <v>120</v>
       </c>
@@ -2260,7 +2260,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2345,7 +2345,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2418,8 +2418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D515F8C6-F732-4239-8790-C00BB6FBEA93}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2430,18 +2430,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="F2" t="s">
         <v>113</v>
       </c>

</xml_diff>